<commit_message>
added q to questions for pandas
</commit_message>
<xml_diff>
--- a/kev/survey_questions.xlsx
+++ b/kev/survey_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevineliasen/GoogleDrive/CodingStuff/Codeup/Capstone/kev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD25F73-5B72-DF48-BBF0-6C9D21E05979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68670388-E288-F441-8AEE-DA37D4031EA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{31CA8657-46A0-9D49-84BF-6461B50EDC7B}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">QuestionList!$A$1:$E$73</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,9 +51,6 @@
     <t>question_text</t>
   </si>
   <si>
-    <t>00</t>
-  </si>
-  <si>
     <t>Survey</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>Entry Id</t>
   </si>
   <si>
-    <t>01a</t>
-  </si>
-  <si>
     <t>Work</t>
   </si>
   <si>
@@ -75,138 +69,63 @@
     <t>Title</t>
   </si>
   <si>
-    <t>01b</t>
-  </si>
-  <si>
     <t>Job Taxo ID</t>
   </si>
   <si>
-    <t>01c</t>
-  </si>
-  <si>
     <t>Job ID</t>
   </si>
   <si>
-    <t>02a</t>
-  </si>
-  <si>
     <t>Research Duties</t>
   </si>
   <si>
     <t>Conducting Research</t>
   </si>
   <si>
-    <t>02b</t>
-  </si>
-  <si>
     <t>Analyzing Research</t>
   </si>
   <si>
-    <t>02c</t>
-  </si>
-  <si>
     <t>Buying Research Reports</t>
   </si>
   <si>
-    <t>02d</t>
-  </si>
-  <si>
     <t>Managing Research Projects</t>
   </si>
   <si>
-    <t>02e</t>
-  </si>
-  <si>
     <t>Observing Research</t>
   </si>
   <si>
-    <t>02f</t>
-  </si>
-  <si>
     <t>Planning Research</t>
   </si>
   <si>
-    <t>02g</t>
-  </si>
-  <si>
     <t>Teaching Research</t>
   </si>
   <si>
-    <t>02h</t>
-  </si>
-  <si>
     <t>Advocating for Research</t>
   </si>
   <si>
-    <t>02i</t>
-  </si>
-  <si>
     <t>Hiring Research Vendors</t>
   </si>
   <si>
-    <t>02j</t>
-  </si>
-  <si>
     <t>Leading a Research Team or Organization</t>
   </si>
   <si>
-    <t>03</t>
-  </si>
-  <si>
     <t>Company Size</t>
   </si>
   <si>
     <t>How many people does your company or organization employ?</t>
   </si>
   <si>
-    <t>04</t>
-  </si>
-  <si>
     <t>Company researchers</t>
   </si>
   <si>
     <t>How many people in your company or organization have research as part of their role?</t>
   </si>
   <si>
-    <t>08a</t>
-  </si>
-  <si>
     <t>Experience</t>
   </si>
   <si>
     <t>Research Experience</t>
   </si>
   <si>
-    <t>08b</t>
-  </si>
-  <si>
-    <t>08c</t>
-  </si>
-  <si>
-    <t>08d</t>
-  </si>
-  <si>
-    <t>08e</t>
-  </si>
-  <si>
-    <t>08f</t>
-  </si>
-  <si>
-    <t>08g</t>
-  </si>
-  <si>
-    <t>08h</t>
-  </si>
-  <si>
-    <t>08i</t>
-  </si>
-  <si>
-    <t>08j</t>
-  </si>
-  <si>
-    <t>11a</t>
-  </si>
-  <si>
     <t>Learning</t>
   </si>
   <si>
@@ -216,75 +135,36 @@
     <t>Watch videos of talks</t>
   </si>
   <si>
-    <t>11b</t>
-  </si>
-  <si>
     <t>Read blogs and/or books</t>
   </si>
   <si>
-    <t>11c</t>
-  </si>
-  <si>
     <t>Attend a local meetup or talk</t>
   </si>
   <si>
-    <t>11d</t>
-  </si>
-  <si>
     <t>Attend a longer form workshop</t>
   </si>
   <si>
-    <t>11e</t>
-  </si>
-  <si>
     <t>Attend a conference</t>
   </si>
   <si>
-    <t>12a</t>
-  </si>
-  <si>
     <t>How You Want to Learn</t>
   </si>
   <si>
     <t>Watch a video of a talk</t>
   </si>
   <si>
-    <t>12b</t>
-  </si>
-  <si>
     <t>Read a blog post or Medium article</t>
   </si>
   <si>
-    <t>12c</t>
-  </si>
-  <si>
     <t>Read a book</t>
   </si>
   <si>
-    <t>12d</t>
-  </si>
-  <si>
     <t>Ask in a LinkedIn group, Slack channel, or mailing list</t>
   </si>
   <si>
-    <t>12e</t>
-  </si>
-  <si>
     <t>Ask a colleague or manager or mentor</t>
   </si>
   <si>
-    <t>12f</t>
-  </si>
-  <si>
-    <t>12g</t>
-  </si>
-  <si>
-    <t>12h</t>
-  </si>
-  <si>
-    <t>13a</t>
-  </si>
-  <si>
     <t>Conference 1</t>
   </si>
   <si>
@@ -294,63 +174,33 @@
     <t>Speakers you've heard of</t>
   </si>
   <si>
-    <t>13b</t>
-  </si>
-  <si>
     <t>Diversity of speakers' backgrounds and perspectives</t>
   </si>
   <si>
-    <t>13c</t>
-  </si>
-  <si>
     <t>Topics covered</t>
   </si>
   <si>
-    <t>13d</t>
-  </si>
-  <si>
     <t>Format of sessions</t>
   </si>
   <si>
-    <t>13e</t>
-  </si>
-  <si>
     <t>Networking opportunities</t>
   </si>
   <si>
-    <t>13g</t>
-  </si>
-  <si>
     <t>Variety of attendees to network with</t>
   </si>
   <si>
-    <t>13h</t>
-  </si>
-  <si>
     <t>Code of conduct in place</t>
   </si>
   <si>
-    <t>13i</t>
-  </si>
-  <si>
     <t>Conference location</t>
   </si>
   <si>
-    <t>13j</t>
-  </si>
-  <si>
     <t>Your (or your employer's) ability to pay</t>
   </si>
   <si>
-    <t>13f</t>
-  </si>
-  <si>
     <t>Number of attendees/degree of intimacy</t>
   </si>
   <si>
-    <t>19a</t>
-  </si>
-  <si>
     <t>Conference 2</t>
   </si>
   <si>
@@ -360,178 +210,328 @@
     <t>Keynotes from leaders in research</t>
   </si>
   <si>
-    <t>19b</t>
-  </si>
-  <si>
     <t>Full length talks (30-60 minutes)</t>
   </si>
   <si>
-    <t>19c</t>
-  </si>
-  <si>
     <t>Short or Lightning talks (&lt; 30 minutes)</t>
   </si>
   <si>
-    <t>19d</t>
-  </si>
-  <si>
     <t>Workshops</t>
   </si>
   <si>
-    <t>19e</t>
-  </si>
-  <si>
     <t>Networking events</t>
   </si>
   <si>
-    <t>19f</t>
-  </si>
-  <si>
     <t>Social events (e.g., parties, karaoke, game night)</t>
   </si>
   <si>
-    <t>19g</t>
-  </si>
-  <si>
     <t>Q&amp;A/AMA (ask me anything) sessions</t>
   </si>
   <si>
-    <t>19h</t>
-  </si>
-  <si>
     <t>Discussion circles/topic tables</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>Sessions of Interest</t>
   </si>
   <si>
     <t>Did we miss any other types of conference sessions that you'd like to mention?</t>
   </si>
   <si>
-    <t>05</t>
-  </si>
-  <si>
     <t>Industry</t>
   </si>
   <si>
     <t>What is your company or organization's primary industry (e.g., fintech, healthcare)?</t>
   </si>
   <si>
-    <t>06</t>
-  </si>
-  <si>
     <t>Current Research</t>
   </si>
   <si>
     <t>What types of research do you (or your  team) currently use to make decisions?</t>
   </si>
   <si>
-    <t>07</t>
-  </si>
-  <si>
     <t>Future Research</t>
   </si>
   <si>
     <t>What types of research are you (or your  team) considering using in the future?</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>Describe your educational background with research (e.g., you took classes, participated in running studies, majored in a research-related area).</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>Event Selection</t>
   </si>
   <si>
     <t>How do you decide which events to attend? (If travel is a consideration, how so?)</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>Best Event</t>
   </si>
   <si>
     <t>What was the best professional learning event experience you've ever had? What made it great?</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>Events Attended</t>
   </si>
   <si>
     <t>What (if any) events have you attended on the subject of research in the past few years?</t>
   </si>
   <si>
-    <t>17a</t>
-  </si>
-  <si>
     <t>Desired Size</t>
   </si>
   <si>
     <t>What would be the ideal audience size for a conference about research that *you* would want to attend?</t>
   </si>
   <si>
-    <t>17b</t>
-  </si>
-  <si>
     <t>Desired Size Cat</t>
   </si>
   <si>
     <t>Ideal Audience Size (Standardized)</t>
   </si>
   <si>
-    <t>18a</t>
-  </si>
-  <si>
     <t>Desired Structure</t>
   </si>
   <si>
     <t>What would be the ideal structure for a conference about research that *you* would want to attend?</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>Desired Topics</t>
   </si>
   <si>
     <t>If attending a conference about research, what subjects would *you* most want to see covered?</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>Desired Attendees</t>
   </si>
   <si>
     <t>If attending a conference about research, who might you be excited to see there (e.g., types of people, specific individuals, organizations)?</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>Conference Advice</t>
   </si>
   <si>
     <t>Let’s say (hypothetically of course) that Rosenfeld Media was exploring the idea of a conference about research. What advice would you give us?</t>
   </si>
   <si>
-    <t>09a</t>
-  </si>
-  <si>
     <t>Did any part of your education include learning about how to conduct research?</t>
   </si>
   <si>
     <t>Research Education</t>
+  </si>
+  <si>
+    <t>q00</t>
+  </si>
+  <si>
+    <t>q01a</t>
+  </si>
+  <si>
+    <t>q01b</t>
+  </si>
+  <si>
+    <t>q01c</t>
+  </si>
+  <si>
+    <t>q02a</t>
+  </si>
+  <si>
+    <t>q02b</t>
+  </si>
+  <si>
+    <t>q02c</t>
+  </si>
+  <si>
+    <t>q02d</t>
+  </si>
+  <si>
+    <t>q02e</t>
+  </si>
+  <si>
+    <t>q02f</t>
+  </si>
+  <si>
+    <t>q02g</t>
+  </si>
+  <si>
+    <t>q02h</t>
+  </si>
+  <si>
+    <t>q02i</t>
+  </si>
+  <si>
+    <t>q02j</t>
+  </si>
+  <si>
+    <t>q03</t>
+  </si>
+  <si>
+    <t>q04</t>
+  </si>
+  <si>
+    <t>q05</t>
+  </si>
+  <si>
+    <t>q06</t>
+  </si>
+  <si>
+    <t>q07</t>
+  </si>
+  <si>
+    <t>q08a</t>
+  </si>
+  <si>
+    <t>q08b</t>
+  </si>
+  <si>
+    <t>q08c</t>
+  </si>
+  <si>
+    <t>q08d</t>
+  </si>
+  <si>
+    <t>q08e</t>
+  </si>
+  <si>
+    <t>q08f</t>
+  </si>
+  <si>
+    <t>q08g</t>
+  </si>
+  <si>
+    <t>q08h</t>
+  </si>
+  <si>
+    <t>q08i</t>
+  </si>
+  <si>
+    <t>q08j</t>
+  </si>
+  <si>
+    <t>q09a</t>
+  </si>
+  <si>
+    <t>q10</t>
+  </si>
+  <si>
+    <t>q11a</t>
+  </si>
+  <si>
+    <t>q11b</t>
+  </si>
+  <si>
+    <t>q11c</t>
+  </si>
+  <si>
+    <t>q11d</t>
+  </si>
+  <si>
+    <t>q11e</t>
+  </si>
+  <si>
+    <t>q12a</t>
+  </si>
+  <si>
+    <t>q12b</t>
+  </si>
+  <si>
+    <t>q12c</t>
+  </si>
+  <si>
+    <t>q12d</t>
+  </si>
+  <si>
+    <t>q12e</t>
+  </si>
+  <si>
+    <t>q12f</t>
+  </si>
+  <si>
+    <t>q12g</t>
+  </si>
+  <si>
+    <t>q12h</t>
+  </si>
+  <si>
+    <t>q13a</t>
+  </si>
+  <si>
+    <t>q13b</t>
+  </si>
+  <si>
+    <t>q13c</t>
+  </si>
+  <si>
+    <t>q13d</t>
+  </si>
+  <si>
+    <t>q13e</t>
+  </si>
+  <si>
+    <t>q13f</t>
+  </si>
+  <si>
+    <t>q13g</t>
+  </si>
+  <si>
+    <t>q13h</t>
+  </si>
+  <si>
+    <t>q13i</t>
+  </si>
+  <si>
+    <t>q13j</t>
+  </si>
+  <si>
+    <t>q14</t>
+  </si>
+  <si>
+    <t>q15</t>
+  </si>
+  <si>
+    <t>q16</t>
+  </si>
+  <si>
+    <t>q17a</t>
+  </si>
+  <si>
+    <t>q17b</t>
+  </si>
+  <si>
+    <t>q18a</t>
+  </si>
+  <si>
+    <t>q19a</t>
+  </si>
+  <si>
+    <t>q19b</t>
+  </si>
+  <si>
+    <t>q19c</t>
+  </si>
+  <si>
+    <t>q19d</t>
+  </si>
+  <si>
+    <t>q19e</t>
+  </si>
+  <si>
+    <t>q19f</t>
+  </si>
+  <si>
+    <t>q19g</t>
+  </si>
+  <si>
+    <t>q19h</t>
+  </si>
+  <si>
+    <t>q20</t>
+  </si>
+  <si>
+    <t>q21</t>
+  </si>
+  <si>
+    <t>q22</t>
+  </si>
+  <si>
+    <t>q23</t>
   </si>
 </sst>
 </file>
@@ -883,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53992D9E-FAE0-004A-B683-F804D396F232}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -915,1226 +915,1226 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>18</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>127</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>71</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>133</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>123</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>164</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>135</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>129</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D37" t="b">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>139</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C50" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C51" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C54" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C55" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C56" t="s">
-        <v>137</v>
+        <v>74</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B57" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C57" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C58" t="s">
-        <v>143</v>
+        <v>78</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>144</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B59" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C59" t="s">
-        <v>146</v>
+        <v>80</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>147</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C60" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>150</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B61" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C61" t="s">
-        <v>152</v>
+        <v>84</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>153</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>104</v>
+        <v>154</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C62" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D62" t="b">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C63" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>110</v>
+        <v>156</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C64" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D64" t="b">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="B65" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C65" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>113</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="B66" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C66" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D66" t="b">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="B67" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C67" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C68" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D68" t="b">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="B69" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C69" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D69" t="b">
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>121</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="B70" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C70" t="s">
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C71" t="s">
-        <v>155</v>
+        <v>86</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>156</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B72" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C72" t="s">
-        <v>158</v>
+        <v>88</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B73" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C73" t="s">
-        <v>161</v>
+        <v>90</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>162</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of python short-hand names for variables
</commit_message>
<xml_diff>
--- a/kev/survey_questions.xlsx
+++ b/kev/survey_questions.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevineliasen/GoogleDrive/CodingStuff/Codeup/Capstone/kev/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanoslin/codeup-data-science/Capstone/kev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68670388-E288-F441-8AEE-DA37D4031EA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A898C0-BB2D-504E-B528-95AA7654B521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{31CA8657-46A0-9D49-84BF-6461B50EDC7B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{31CA8657-46A0-9D49-84BF-6461B50EDC7B}"/>
   </bookViews>
   <sheets>
     <sheet name="QuestionList" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">QuestionList!$A$1:$E$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">QuestionList!$A$1:$F$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="239">
   <si>
     <t>QID2</t>
   </si>
@@ -532,6 +532,225 @@
   </si>
   <si>
     <t>q23</t>
+  </si>
+  <si>
+    <t>resp_id</t>
+  </si>
+  <si>
+    <t>job_title</t>
+  </si>
+  <si>
+    <t>job_taxo</t>
+  </si>
+  <si>
+    <t>job_id</t>
+  </si>
+  <si>
+    <t>num_employees</t>
+  </si>
+  <si>
+    <t>num_researchers</t>
+  </si>
+  <si>
+    <t>types_res_used</t>
+  </si>
+  <si>
+    <t>future_res</t>
+  </si>
+  <si>
+    <t>job_conduct_res</t>
+  </si>
+  <si>
+    <t>job_analyze_res</t>
+  </si>
+  <si>
+    <t>job_buy_res_report</t>
+  </si>
+  <si>
+    <t>job_manage_res_proj</t>
+  </si>
+  <si>
+    <t>job_observe_res</t>
+  </si>
+  <si>
+    <t>job_plan_res</t>
+  </si>
+  <si>
+    <t>job_teach_res</t>
+  </si>
+  <si>
+    <t>job_advocate_res</t>
+  </si>
+  <si>
+    <t>job_hire_res_vendor</t>
+  </si>
+  <si>
+    <t>job_lead_res_team</t>
+  </si>
+  <si>
+    <t>primary_industry</t>
+  </si>
+  <si>
+    <t>exp_conduct_res</t>
+  </si>
+  <si>
+    <t>exp_analyze_res</t>
+  </si>
+  <si>
+    <t>exp_buy_res_report</t>
+  </si>
+  <si>
+    <t>exp_manage_res_proj</t>
+  </si>
+  <si>
+    <t>exp_observe_res</t>
+  </si>
+  <si>
+    <t>exp_plan_res</t>
+  </si>
+  <si>
+    <t>exp_teach_res</t>
+  </si>
+  <si>
+    <t>exp_advocate_res</t>
+  </si>
+  <si>
+    <t>exp_hire_res_vendor</t>
+  </si>
+  <si>
+    <t>exp_lead_res_team</t>
+  </si>
+  <si>
+    <t>ur_ed_include_res</t>
+  </si>
+  <si>
+    <t>ur_ed_with_res</t>
+  </si>
+  <si>
+    <t>learning_talks</t>
+  </si>
+  <si>
+    <t>learning_read</t>
+  </si>
+  <si>
+    <t>learning_meetup</t>
+  </si>
+  <si>
+    <t>learning_workshop</t>
+  </si>
+  <si>
+    <t>learning_conference</t>
+  </si>
+  <si>
+    <t>likely_watch_video</t>
+  </si>
+  <si>
+    <t>likely_internet</t>
+  </si>
+  <si>
+    <t>likely_book</t>
+  </si>
+  <si>
+    <t>likely_online_group</t>
+  </si>
+  <si>
+    <t>likely_colleague</t>
+  </si>
+  <si>
+    <t>likely_meetup</t>
+  </si>
+  <si>
+    <t>likely_conference</t>
+  </si>
+  <si>
+    <t>likely_workshop</t>
+  </si>
+  <si>
+    <t>factor_speaker</t>
+  </si>
+  <si>
+    <t>factor_diverse_speak</t>
+  </si>
+  <si>
+    <t>factor_topics</t>
+  </si>
+  <si>
+    <t>factor_format_sessions</t>
+  </si>
+  <si>
+    <t>factor_size</t>
+  </si>
+  <si>
+    <t>factor_network</t>
+  </si>
+  <si>
+    <t>factor_variety_attend</t>
+  </si>
+  <si>
+    <t>factor_code</t>
+  </si>
+  <si>
+    <t>factor_location</t>
+  </si>
+  <si>
+    <t>factor_ability_to_pay</t>
+  </si>
+  <si>
+    <t>how_pick_events</t>
+  </si>
+  <si>
+    <t>best_event</t>
+  </si>
+  <si>
+    <t>events_attend_recent</t>
+  </si>
+  <si>
+    <t>ideal_structure</t>
+  </si>
+  <si>
+    <t>session_keynote</t>
+  </si>
+  <si>
+    <t>session_short_talk</t>
+  </si>
+  <si>
+    <t>session_long_talk</t>
+  </si>
+  <si>
+    <t>session_workshop</t>
+  </si>
+  <si>
+    <t>session_network</t>
+  </si>
+  <si>
+    <t>session_social_event</t>
+  </si>
+  <si>
+    <t>session_qa</t>
+  </si>
+  <si>
+    <t>sesson_topic_tables</t>
+  </si>
+  <si>
+    <t>ideal_attendee_size_likert</t>
+  </si>
+  <si>
+    <t>ideal_attendee_size_text</t>
+  </si>
+  <si>
+    <t>other_conference_types</t>
+  </si>
+  <si>
+    <t>ur_prefer_res_topics</t>
+  </si>
+  <si>
+    <t>who_u_want_to_see</t>
+  </si>
+  <si>
+    <t>ur_advice</t>
+  </si>
+  <si>
+    <t>python_name</t>
   </si>
 </sst>
 </file>
@@ -881,1266 +1100,1486 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53992D9E-FAE0-004A-B683-F804D396F232}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" customWidth="1"/>
-    <col min="5" max="5" width="115.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="115.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>238</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>94</v>
       </c>
       <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>95</v>
       </c>
       <c r="B3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>96</v>
       </c>
       <c r="B4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>97</v>
       </c>
       <c r="B5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>98</v>
       </c>
       <c r="B6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>99</v>
       </c>
       <c r="B7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>100</v>
       </c>
       <c r="B8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>101</v>
       </c>
       <c r="B9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>102</v>
       </c>
       <c r="B10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>103</v>
       </c>
       <c r="B11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>104</v>
       </c>
       <c r="B12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>105</v>
       </c>
       <c r="B13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>106</v>
       </c>
       <c r="B14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>107</v>
       </c>
       <c r="B15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>108</v>
       </c>
       <c r="B16" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>24</v>
       </c>
-      <c r="D16" t="b">
+      <c r="E16" t="b">
         <v>0</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>109</v>
       </c>
       <c r="B17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>26</v>
       </c>
-      <c r="D17" t="b">
+      <c r="E17" t="b">
         <v>0</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>110</v>
       </c>
       <c r="B18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C18" t="s">
         <v>8</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>67</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>111</v>
       </c>
       <c r="B19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>69</v>
       </c>
-      <c r="D19" t="b">
+      <c r="E19" t="b">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>112</v>
       </c>
       <c r="B20" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" t="s">
         <v>8</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>71</v>
       </c>
-      <c r="D20" t="b">
+      <c r="E20" t="b">
         <v>0</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>113</v>
       </c>
       <c r="B21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21" t="s">
         <v>28</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>29</v>
       </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>114</v>
       </c>
       <c r="B22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" t="s">
         <v>28</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>29</v>
       </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>115</v>
       </c>
       <c r="B23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C23" t="s">
         <v>28</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>29</v>
       </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>116</v>
       </c>
       <c r="B24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C24" t="s">
         <v>28</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>29</v>
       </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>117</v>
       </c>
       <c r="B25" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>29</v>
       </c>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>118</v>
       </c>
       <c r="B26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C26" t="s">
         <v>28</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>29</v>
       </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>119</v>
       </c>
       <c r="B27" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" t="s">
         <v>28</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>29</v>
       </c>
-      <c r="D27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>120</v>
       </c>
       <c r="B28" t="s">
+        <v>192</v>
+      </c>
+      <c r="C28" t="s">
         <v>28</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>29</v>
       </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>121</v>
       </c>
       <c r="B29" t="s">
+        <v>193</v>
+      </c>
+      <c r="C29" t="s">
         <v>28</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>29</v>
       </c>
-      <c r="D29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>122</v>
       </c>
       <c r="B30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C30" t="s">
         <v>28</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>29</v>
       </c>
-      <c r="D30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>123</v>
       </c>
       <c r="B31" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" t="s">
         <v>28</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>93</v>
       </c>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>124</v>
       </c>
       <c r="B32" t="s">
+        <v>196</v>
+      </c>
+      <c r="C32" t="s">
         <v>28</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>93</v>
       </c>
-      <c r="D32" t="b">
+      <c r="E32" t="b">
         <v>0</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>125</v>
       </c>
       <c r="B33" t="s">
+        <v>197</v>
+      </c>
+      <c r="C33" t="s">
         <v>30</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>31</v>
       </c>
-      <c r="D33" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>126</v>
       </c>
       <c r="B34" t="s">
+        <v>198</v>
+      </c>
+      <c r="C34" t="s">
         <v>30</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>31</v>
       </c>
-      <c r="D34" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>127</v>
       </c>
       <c r="B35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C35" t="s">
         <v>30</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>31</v>
       </c>
-      <c r="D35" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>128</v>
       </c>
       <c r="B36" t="s">
+        <v>200</v>
+      </c>
+      <c r="C36" t="s">
         <v>30</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>31</v>
       </c>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>129</v>
       </c>
       <c r="B37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" t="s">
         <v>30</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>31</v>
       </c>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>130</v>
       </c>
       <c r="B38" t="s">
+        <v>202</v>
+      </c>
+      <c r="C38" t="s">
         <v>30</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>37</v>
       </c>
-      <c r="D38" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>131</v>
       </c>
       <c r="B39" t="s">
+        <v>203</v>
+      </c>
+      <c r="C39" t="s">
         <v>30</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>37</v>
       </c>
-      <c r="D39" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>132</v>
       </c>
       <c r="B40" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" t="s">
         <v>30</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>37</v>
       </c>
-      <c r="D40" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>133</v>
       </c>
       <c r="B41" t="s">
+        <v>205</v>
+      </c>
+      <c r="C41" t="s">
         <v>30</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>37</v>
       </c>
-      <c r="D41" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>134</v>
       </c>
       <c r="B42" t="s">
+        <v>206</v>
+      </c>
+      <c r="C42" t="s">
         <v>30</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>37</v>
       </c>
-      <c r="D42" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>135</v>
       </c>
       <c r="B43" t="s">
+        <v>207</v>
+      </c>
+      <c r="C43" t="s">
         <v>30</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>37</v>
       </c>
-      <c r="D43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>136</v>
       </c>
       <c r="B44" t="s">
+        <v>208</v>
+      </c>
+      <c r="C44" t="s">
         <v>30</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>37</v>
       </c>
-      <c r="D44" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>137</v>
       </c>
       <c r="B45" t="s">
+        <v>209</v>
+      </c>
+      <c r="C45" t="s">
         <v>30</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>37</v>
       </c>
-      <c r="D45" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>138</v>
       </c>
       <c r="B46" t="s">
+        <v>210</v>
+      </c>
+      <c r="C46" t="s">
         <v>43</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>44</v>
       </c>
-      <c r="D46" t="b">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>139</v>
       </c>
       <c r="B47" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" t="s">
         <v>43</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>44</v>
       </c>
-      <c r="D47" t="b">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>140</v>
       </c>
       <c r="B48" t="s">
+        <v>212</v>
+      </c>
+      <c r="C48" t="s">
         <v>43</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>44</v>
       </c>
-      <c r="D48" t="b">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>141</v>
       </c>
       <c r="B49" t="s">
+        <v>213</v>
+      </c>
+      <c r="C49" t="s">
         <v>43</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>44</v>
       </c>
-      <c r="D49" t="b">
-        <v>1</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>142</v>
       </c>
       <c r="B50" t="s">
+        <v>214</v>
+      </c>
+      <c r="C50" t="s">
         <v>43</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>44</v>
       </c>
-      <c r="D50" t="b">
-        <v>1</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>143</v>
       </c>
       <c r="B51" t="s">
+        <v>215</v>
+      </c>
+      <c r="C51" t="s">
         <v>43</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>44</v>
       </c>
-      <c r="D51" t="b">
-        <v>1</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>144</v>
       </c>
       <c r="B52" t="s">
+        <v>216</v>
+      </c>
+      <c r="C52" t="s">
         <v>43</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>44</v>
       </c>
-      <c r="D52" t="b">
-        <v>1</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>145</v>
       </c>
       <c r="B53" t="s">
+        <v>217</v>
+      </c>
+      <c r="C53" t="s">
         <v>43</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>44</v>
       </c>
-      <c r="D53" t="b">
-        <v>1</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="E53" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>146</v>
       </c>
       <c r="B54" t="s">
+        <v>218</v>
+      </c>
+      <c r="C54" t="s">
         <v>43</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>44</v>
       </c>
-      <c r="D54" t="b">
-        <v>1</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>147</v>
       </c>
       <c r="B55" t="s">
+        <v>219</v>
+      </c>
+      <c r="C55" t="s">
         <v>43</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>44</v>
       </c>
-      <c r="D55" t="b">
-        <v>1</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="E55" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>148</v>
       </c>
       <c r="B56" t="s">
+        <v>220</v>
+      </c>
+      <c r="C56" t="s">
         <v>43</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>74</v>
       </c>
-      <c r="D56" t="b">
+      <c r="E56" t="b">
         <v>0</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>149</v>
       </c>
       <c r="B57" t="s">
+        <v>221</v>
+      </c>
+      <c r="C57" t="s">
         <v>43</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>76</v>
       </c>
-      <c r="D57" t="b">
+      <c r="E57" t="b">
         <v>0</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>150</v>
       </c>
       <c r="B58" t="s">
+        <v>222</v>
+      </c>
+      <c r="C58" t="s">
         <v>43</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>78</v>
       </c>
-      <c r="D58" t="b">
+      <c r="E58" t="b">
         <v>0</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>151</v>
       </c>
       <c r="B59" t="s">
+        <v>232</v>
+      </c>
+      <c r="C59" t="s">
         <v>55</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>80</v>
       </c>
-      <c r="D59" t="b">
-        <v>1</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="E59" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>152</v>
       </c>
       <c r="B60" t="s">
+        <v>233</v>
+      </c>
+      <c r="C60" t="s">
         <v>55</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>82</v>
       </c>
-      <c r="D60" t="b">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="E60" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>153</v>
       </c>
       <c r="B61" t="s">
+        <v>223</v>
+      </c>
+      <c r="C61" t="s">
         <v>55</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>84</v>
       </c>
-      <c r="D61" t="b">
-        <v>1</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="E61" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>154</v>
       </c>
       <c r="B62" t="s">
+        <v>224</v>
+      </c>
+      <c r="C62" t="s">
         <v>55</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>56</v>
       </c>
-      <c r="D62" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="E62" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>155</v>
       </c>
       <c r="B63" t="s">
+        <v>226</v>
+      </c>
+      <c r="C63" t="s">
         <v>55</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>56</v>
       </c>
-      <c r="D63" t="b">
-        <v>1</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>156</v>
       </c>
       <c r="B64" t="s">
+        <v>225</v>
+      </c>
+      <c r="C64" t="s">
         <v>55</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>56</v>
       </c>
-      <c r="D64" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" t="s">
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>157</v>
       </c>
       <c r="B65" t="s">
+        <v>227</v>
+      </c>
+      <c r="C65" t="s">
         <v>55</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>56</v>
       </c>
-      <c r="D65" t="b">
-        <v>1</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="E65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>158</v>
       </c>
       <c r="B66" t="s">
+        <v>228</v>
+      </c>
+      <c r="C66" t="s">
         <v>55</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>56</v>
       </c>
-      <c r="D66" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" t="s">
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>159</v>
       </c>
       <c r="B67" t="s">
+        <v>229</v>
+      </c>
+      <c r="C67" t="s">
         <v>55</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>56</v>
       </c>
-      <c r="D67" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" t="s">
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>160</v>
       </c>
       <c r="B68" t="s">
+        <v>230</v>
+      </c>
+      <c r="C68" t="s">
         <v>55</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>56</v>
       </c>
-      <c r="D68" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="E68" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>161</v>
       </c>
       <c r="B69" t="s">
+        <v>231</v>
+      </c>
+      <c r="C69" t="s">
         <v>55</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>56</v>
       </c>
-      <c r="D69" t="b">
-        <v>1</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>162</v>
       </c>
       <c r="B70" t="s">
+        <v>234</v>
+      </c>
+      <c r="C70" t="s">
         <v>55</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>65</v>
       </c>
-      <c r="D70" t="b">
+      <c r="E70" t="b">
         <v>0</v>
       </c>
-      <c r="E70" t="s">
+      <c r="F70" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>163</v>
       </c>
       <c r="B71" t="s">
+        <v>235</v>
+      </c>
+      <c r="C71" t="s">
         <v>55</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>86</v>
       </c>
-      <c r="D71" t="b">
+      <c r="E71" t="b">
         <v>0</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>164</v>
       </c>
       <c r="B72" t="s">
+        <v>236</v>
+      </c>
+      <c r="C72" t="s">
         <v>55</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>88</v>
       </c>
-      <c r="D72" t="b">
+      <c r="E72" t="b">
         <v>0</v>
       </c>
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>165</v>
       </c>
       <c r="B73" t="s">
+        <v>237</v>
+      </c>
+      <c r="C73" t="s">
         <v>55</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>90</v>
       </c>
-      <c r="D73" t="b">
+      <c r="E73" t="b">
         <v>0</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E73" xr:uid="{4CB6D847-279A-B844-8D45-D48098ACB70C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E73">
-      <sortCondition ref="A2:A73"/>
+  <autoFilter ref="A1:F73" xr:uid="{4CB6D847-279A-B844-8D45-D48098ACB70C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F74">
+      <sortCondition ref="A2:A74"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>